<commit_message>
First run on Namyeon's computer
</commit_message>
<xml_diff>
--- a/Output/PBL/Customer/Air_Force/Air_Force_Contracts.xlsx
+++ b/Output/PBL/Customer/Air_Force/Air_Force_Contracts.xlsx
@@ -189,10 +189,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="171" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="172" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="168" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="174" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="175" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="173" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="176" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -230,10 +230,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>